<commit_message>
3.1 Example 2 output from YAML now matches that from CTI.
</commit_message>
<xml_diff>
--- a/PEUQSE/simulationDriver_YAML/ceO2_output_rates_gas_CTI.xlsx
+++ b/PEUQSE/simulationDriver_YAML/ceO2_output_rates_gas_CTI.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\PEUQSE\PEUQSE\simulationDriver_YAML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{37951F89-BC25-40F2-A25E-DB1AB07CADCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816102BF-6491-4B6B-8AD1-7DE9EA3B8E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ceO2_output_rates_gas" sheetId="1" r:id="rId1"/>
+    <sheet name="ceO2_output_rates_gas_Example2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,7 +628,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ceO2_output_rates_gas!$C$1</c:f>
+              <c:f>ceO2_output_rates_gas_Example2!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -661,7 +661,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ceO2_output_rates_gas!$B$2:$B$501</c:f>
+              <c:f>ceO2_output_rates_gas_Example2!$B$2:$B$501</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="500"/>
@@ -2170,7 +2170,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ceO2_output_rates_gas!$C$2:$C$501</c:f>
+              <c:f>ceO2_output_rates_gas_Example2!$C$2:$C$501</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="500"/>
@@ -4764,11 +4764,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>